<commit_message>
02/01/25 Commit 3 - Optimized the data provider based on the method name or test name for sheet input
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA - Copy.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA - Copy.xlsx
@@ -5,41 +5,42 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajwal\OneDrive - CYBERCORP LIMITED\Projects\intellij-workspace\UEM_AUTOAMATION_V3\src\main\java\com\uem_automation\qa\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cybercorpkolkata-my.sharepoint.com/personal/prajwal_solanke_sundynetech_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="8_{70064AC4-793D-43B6-A904-992B3B16F318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7458357C-01A7-4BB3-978D-4FC47BAF8A3F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DF9A577-392E-4330-80A0-8413EACD350B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="20" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Template" sheetId="2" r:id="rId2"/>
-    <sheet name="802.1x Security" sheetId="5" r:id="rId3"/>
-    <sheet name="Computer Name" sheetId="4" r:id="rId4"/>
-    <sheet name="Ethernet Setup" sheetId="6" r:id="rId5"/>
-    <sheet name="Wireless Properties" sheetId="7" r:id="rId6"/>
-    <sheet name="Wireless Setup" sheetId="8" r:id="rId7"/>
-    <sheet name="Display Settings" sheetId="9" r:id="rId8"/>
-    <sheet name="Keyboard Settings" sheetId="10" r:id="rId9"/>
-    <sheet name="Mouse Settings" sheetId="11" r:id="rId10"/>
-    <sheet name="Power Option" sheetId="12" r:id="rId11"/>
-    <sheet name="Add Printer" sheetId="13" r:id="rId12"/>
-    <sheet name="Date &amp; Time" sheetId="14" r:id="rId13"/>
-    <sheet name="Region &amp; Location" sheetId="15" r:id="rId14"/>
-    <sheet name="Application Command" sheetId="16" r:id="rId15"/>
-    <sheet name="Environment Variable" sheetId="17" r:id="rId16"/>
-    <sheet name="History Cleaner" sheetId="18" r:id="rId17"/>
-    <sheet name="Registry Backup Restore" sheetId="19" r:id="rId18"/>
-    <sheet name="Startup Application List" sheetId="20" r:id="rId19"/>
-    <sheet name="Task Scheduler" sheetId="21" r:id="rId20"/>
-    <sheet name="Advanced Settings" sheetId="22" r:id="rId21"/>
-    <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId22"/>
-    <sheet name="Change VNC Password" sheetId="25" r:id="rId23"/>
-    <sheet name="General Settings" sheetId="26" r:id="rId24"/>
-    <sheet name="Services" sheetId="27" r:id="rId25"/>
-    <sheet name="USB Device Manager" sheetId="28" r:id="rId26"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId27"/>
+    <sheet name="802xSecurity" sheetId="5" r:id="rId3"/>
+    <sheet name="ComputerName" sheetId="4" r:id="rId4"/>
+    <sheet name="EthernetSetup" sheetId="6" r:id="rId5"/>
+    <sheet name="WirelessProperties" sheetId="7" r:id="rId6"/>
+    <sheet name="WirelessSetup" sheetId="8" r:id="rId7"/>
+    <sheet name="DisplaySettings" sheetId="9" r:id="rId8"/>
+    <sheet name="KeyboardSettings" sheetId="10" r:id="rId9"/>
+    <sheet name="MouseSettings" sheetId="11" r:id="rId10"/>
+    <sheet name="PowerOption" sheetId="12" r:id="rId11"/>
+    <sheet name="AddPrinter" sheetId="13" r:id="rId12"/>
+    <sheet name="DateAndTime" sheetId="14" r:id="rId13"/>
+    <sheet name="RegionAndLocation" sheetId="15" r:id="rId14"/>
+    <sheet name="ApplicationCommand" sheetId="16" r:id="rId15"/>
+    <sheet name="EnvironmentVariable" sheetId="17" r:id="rId16"/>
+    <sheet name="HistoryCleaner" sheetId="18" r:id="rId17"/>
+    <sheet name="RegistryBackupRestore" sheetId="19" r:id="rId18"/>
+    <sheet name="StartupApplicationList" sheetId="20" r:id="rId19"/>
+    <sheet name="TaskScheduler" sheetId="21" r:id="rId20"/>
+    <sheet name="AdvancedSettings" sheetId="22" r:id="rId21"/>
+    <sheet name="ChangeVNCPassword" sheetId="25" r:id="rId22"/>
+    <sheet name="GeneralSettings" sheetId="26" r:id="rId23"/>
+    <sheet name="Services" sheetId="27" r:id="rId24"/>
+    <sheet name="USBDeviceManager" sheetId="28" r:id="rId25"/>
+    <sheet name="UserManagement" sheetId="29" r:id="rId26"/>
+    <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId27"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId28"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="316">
   <si>
     <t>Email</t>
   </si>
@@ -960,16 +961,63 @@
   </si>
   <si>
     <t>Wireless Controllers</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Member Of</t>
+  </si>
+  <si>
+    <t>User Can Not Change The Password</t>
+  </si>
+  <si>
+    <t>Password Never Expires</t>
+  </si>
+  <si>
+    <t>Disable User</t>
+  </si>
+  <si>
+    <t>Add User</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin@123</t>
+  </si>
+  <si>
+    <t>Admin Admin</t>
+  </si>
+  <si>
+    <t>testdata description</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Reset User</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1037,10 +1085,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1061,8 +1110,10 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3141,135 +3192,6 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32692EE9-61EF-4346-8B2E-6D573605C2CE}">
-  <dimension ref="A1:H4"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93683C3E-F6E3-4E2D-A41A-96C24AE51928}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3312,7 +3234,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F76283-0284-477C-A0E1-221B144A3917}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3361,7 +3283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287760A5-7A67-48AD-A225-152416471720}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -3485,12 +3407,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662CFF93-55A6-4800-A79E-B4AD6B76DAB4}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3618,7 +3540,295 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0651430C-B53C-46FF-88EE-C88461C708DA}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{5ABB11AE-16C7-4605-8B8B-4BC057ED356E}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{57DEC2C1-E1BE-4A15-9F09-97C5B18BA42B}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{4CC34BA5-97B0-4876-9642-A3C41A474340}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32692EE9-61EF-4346-8B2E-6D573605C2CE}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFCD414-8863-483B-A9A4-10072CB31342}">
   <dimension ref="A1:K34"/>
   <sheetViews>
@@ -5317,6 +5527,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFE392A59B870547B1C3C655506A654E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c5dcf9363f032dfeeb11d9ad86bb7b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bede5cfa-631d-4fd3-b0c4-59605dda9e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d394e0e01a44c6ec4efd03b5e4dcc17" ns3:_="">
     <xsd:import namespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
@@ -5504,15 +5723,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -5522,6 +5732,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5539,26 +5757,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
03/01/25 Commit - added tc for security
completed TC_TM_027_apply_security_file_system_WriteFilterOperations
completed TC_TM_030_software_deployment_SoftwarePatchInstallUninstall
created master value in excel for template name
added exceptions in the failed test cases
</commit_message>
<xml_diff>
--- a/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA - Copy.xlsx
+++ b/src/main/java/com/uem_automation/qa/testdata/UEM_AUTOMATION_TESTDATA - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cybercorpkolkata-my.sharepoint.com/personal/prajwal_solanke_sundynetech_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DF9A577-392E-4330-80A0-8413EACD350B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{F5CB9422-ACA2-418A-B857-EE9F760A117B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{8CC3C6D7-8AE9-4987-B0A6-C7FE2030C738}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22995" windowHeight="10545" firstSheet="23" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -27,20 +27,22 @@
     <sheet name="AddPrinter" sheetId="13" r:id="rId12"/>
     <sheet name="DateAndTime" sheetId="14" r:id="rId13"/>
     <sheet name="RegionAndLocation" sheetId="15" r:id="rId14"/>
-    <sheet name="ApplicationCommand" sheetId="16" r:id="rId15"/>
-    <sheet name="EnvironmentVariable" sheetId="17" r:id="rId16"/>
-    <sheet name="HistoryCleaner" sheetId="18" r:id="rId17"/>
-    <sheet name="RegistryBackupRestore" sheetId="19" r:id="rId18"/>
-    <sheet name="StartupApplicationList" sheetId="20" r:id="rId19"/>
-    <sheet name="TaskScheduler" sheetId="21" r:id="rId20"/>
-    <sheet name="AdvancedSettings" sheetId="22" r:id="rId21"/>
-    <sheet name="ChangeVNCPassword" sheetId="25" r:id="rId22"/>
-    <sheet name="GeneralSettings" sheetId="26" r:id="rId23"/>
-    <sheet name="Services" sheetId="27" r:id="rId24"/>
-    <sheet name="USBDeviceManager" sheetId="28" r:id="rId25"/>
-    <sheet name="UserManagement" sheetId="29" r:id="rId26"/>
-    <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId27"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId28"/>
+    <sheet name="UserSettings" sheetId="30" r:id="rId15"/>
+    <sheet name="ApplicationCommand" sheetId="16" r:id="rId16"/>
+    <sheet name="EnvironmentVariable" sheetId="17" r:id="rId17"/>
+    <sheet name="HistoryCleaner" sheetId="18" r:id="rId18"/>
+    <sheet name="RegistryBackupRestore" sheetId="19" r:id="rId19"/>
+    <sheet name="StartupApplicationList" sheetId="20" r:id="rId20"/>
+    <sheet name="TaskScheduler" sheetId="21" r:id="rId21"/>
+    <sheet name="AdvancedSettings" sheetId="22" r:id="rId22"/>
+    <sheet name="ChangeVNCPassword" sheetId="25" r:id="rId23"/>
+    <sheet name="GeneralSettings" sheetId="26" r:id="rId24"/>
+    <sheet name="Services" sheetId="27" r:id="rId25"/>
+    <sheet name="USBDeviceManager" sheetId="28" r:id="rId26"/>
+    <sheet name="UserManagement" sheetId="29" r:id="rId27"/>
+    <sheet name="WriteFilterOperations" sheetId="32" r:id="rId28"/>
+    <sheet name="SoftwarePatchInstallUninstall" sheetId="24" r:id="rId29"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId30"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="334">
   <si>
     <t>Email</t>
   </si>
@@ -1000,6 +1002,60 @@
   </si>
   <si>
     <t>Reset User</t>
+  </si>
+  <si>
+    <t>Write Filter Setting</t>
+  </si>
+  <si>
+    <t>Write Filter</t>
+  </si>
+  <si>
+    <t>File And Folder Path</t>
+  </si>
+  <si>
+    <t>Registry Path</t>
+  </si>
+  <si>
+    <t>Set Max Cache Size For Next Session</t>
+  </si>
+  <si>
+    <t>Overlay Size</t>
+  </si>
+  <si>
+    <t>Alert User</t>
+  </si>
+  <si>
+    <t>Message Important</t>
+  </si>
+  <si>
+    <t>Disable Write Filter</t>
+  </si>
+  <si>
+    <t>Write Filter Exclusion List</t>
+  </si>
+  <si>
+    <t>Enable UWF</t>
+  </si>
+  <si>
+    <t>testdata</t>
+  </si>
+  <si>
+    <t>testmessage</t>
+  </si>
+  <si>
+    <t>Important</t>
+  </si>
+  <si>
+    <t>Message from Administrator</t>
+  </si>
+  <si>
+    <t>A maintenance task is going to be performed on your desktop. Your device may Shutdown to complete the task, so you need to save any open work to avoid data loss and then press ok</t>
+  </si>
+  <si>
+    <t>FBWF Cache Size</t>
+  </si>
+  <si>
+    <t>Overlay Settings</t>
   </si>
 </sst>
 </file>
@@ -1986,7 +2042,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,6 +2141,39 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990357BF-34A2-47B3-BEE2-914E91C537BD}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D0C37E1-55E4-49D2-90EA-9D4D43D48B78}">
   <dimension ref="A1:M6"/>
   <sheetViews>
@@ -2357,7 +2446,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F766D96-72E8-4C23-B0B5-67E2AEA36DB5}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2399,7 +2488,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47979A52-AC7D-48A2-A130-CC6D77928906}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
@@ -2646,7 +2735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C36428-63BD-472E-9AEF-E7AD7E6DF397}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2727,69 +2816,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C593A65-72D5-488B-B99F-1E676D8D6A63}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2879,6 +2905,69 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C593A65-72D5-488B-B99F-1E676D8D6A63}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE19630C-EDE5-4BC4-9116-6FE0D3ED4CB9}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2928,7 +3017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D193770-0DE9-4AFF-A9CD-47CBE6D06952}">
   <dimension ref="A1:X3"/>
   <sheetViews>
@@ -3191,7 +3280,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93683C3E-F6E3-4E2D-A41A-96C24AE51928}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3234,7 +3323,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F76283-0284-477C-A0E1-221B144A3917}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3283,7 +3372,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287760A5-7A67-48AD-A225-152416471720}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -3407,7 +3496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662CFF93-55A6-4800-A79E-B4AD6B76DAB4}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -3540,7 +3629,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0651430C-B53C-46FF-88EE-C88461C708DA}">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -3699,12 +3788,263 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7878CC6-FA40-4D94-9C3C-EEB0F9DD79C6}">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1021</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1021</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32692EE9-61EF-4346-8B2E-6D573605C2CE}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3828,774 +4168,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFCD414-8863-483B-A9A4-10072CB31342}">
-  <dimension ref="A1:K34"/>
-  <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:H34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="4">
-        <v>0</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="4">
-        <v>2</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="4">
-        <v>3</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="4">
-        <v>13</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="1">
-        <v>802</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="1">
-        <v>802</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="1">
-        <v>802</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H27" s="1">
-        <v>92000</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C82663CF-5C72-4665-9470-E0679D0A24EB}">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4786,6 +4364,768 @@
       </c>
       <c r="K5" s="1" t="s">
         <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFCD414-8863-483B-A9A4-10072CB31342}">
+  <dimension ref="A1:K34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" zoomScale="130" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="4">
+        <v>0</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="4">
+        <v>3</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="4">
+        <v>13</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="1">
+        <v>802</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="1">
+        <v>802</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="1">
+        <v>802</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H27" s="1">
+        <v>92000</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -5527,15 +5867,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFE392A59B870547B1C3C655506A654E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c5dcf9363f032dfeeb11d9ad86bb7b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bede5cfa-631d-4fd3-b0c4-59605dda9e90" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d394e0e01a44c6ec4efd03b5e4dcc17" ns3:_="">
     <xsd:import namespace="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
@@ -5723,7 +6054,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_activity xmlns="bede5cfa-631d-4fd3-b0c4-59605dda9e90" xsi:nil="true"/>
@@ -5731,15 +6062,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1115A243-C08D-40EF-8182-B46E18220BEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5757,18 +6089,26 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0FBC653-3026-41A1-A0E4-1AA0FF7A869E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="bede5cfa-631d-4fd3-b0c4-59605dda9e90"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAE7CF42-BD80-4F72-A4A5-E57C8D02DBB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>